<commit_message>
Agregado SAILE y VIACONSUMO
</commit_message>
<xml_diff>
--- a/Data_rechazos_historicos.xlsx
+++ b/Data_rechazos_historicos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="27">
   <si>
     <t>Distribuidora</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>OSORIO</t>
+  </si>
+  <si>
+    <t>SAILE</t>
+  </si>
+  <si>
+    <t>VIACONSUMO</t>
   </si>
 </sst>
 </file>
@@ -154,8 +160,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B3:G40" totalsRowShown="0">
-  <autoFilter ref="B3:G40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B3:G61" totalsRowShown="0">
+  <autoFilter ref="B3:G61"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Distribuidora"/>
     <tableColumn id="2" name="MES"/>
@@ -431,7 +437,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G40"/>
+  <dimension ref="B3:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1204,6 +1210,426 @@
         <v>10158.85</v>
       </c>
     </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41">
+        <v>224</v>
+      </c>
+      <c r="E41">
+        <v>7</v>
+      </c>
+      <c r="F41">
+        <v>109724.12</v>
+      </c>
+      <c r="G41">
+        <v>562.20000000000005</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42">
+        <v>1111</v>
+      </c>
+      <c r="E42">
+        <v>9</v>
+      </c>
+      <c r="F42">
+        <v>443737.68</v>
+      </c>
+      <c r="G42">
+        <v>876.61</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43">
+        <v>1009</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>370738.75</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44">
+        <v>2069</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>848209.07</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45">
+        <v>2415</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>1314661.01</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46">
+        <v>2386</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>1688685.77</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47">
+        <v>2990</v>
+      </c>
+      <c r="E47">
+        <v>309</v>
+      </c>
+      <c r="F47">
+        <v>3145354.56</v>
+      </c>
+      <c r="G47">
+        <v>55902.06</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D48">
+        <v>1656</v>
+      </c>
+      <c r="E48">
+        <v>182</v>
+      </c>
+      <c r="F48">
+        <v>907141.15</v>
+      </c>
+      <c r="G48">
+        <v>36168.019999999997</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49">
+        <v>527</v>
+      </c>
+      <c r="E49">
+        <v>38</v>
+      </c>
+      <c r="F49">
+        <v>71421.14</v>
+      </c>
+      <c r="G49">
+        <v>1937.2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50">
+        <v>4559</v>
+      </c>
+      <c r="E50">
+        <v>916</v>
+      </c>
+      <c r="F50">
+        <v>605252.14969999995</v>
+      </c>
+      <c r="G50">
+        <v>57711.842400000001</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>26</v>
+      </c>
+      <c r="C51" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51">
+        <v>5249</v>
+      </c>
+      <c r="E51">
+        <v>1786</v>
+      </c>
+      <c r="F51">
+        <v>550799.03469999996</v>
+      </c>
+      <c r="G51">
+        <v>120557.68580000001</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52">
+        <v>8169</v>
+      </c>
+      <c r="E52">
+        <v>1429</v>
+      </c>
+      <c r="F52">
+        <v>788979.92740000004</v>
+      </c>
+      <c r="G52">
+        <v>100371.8541</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>26</v>
+      </c>
+      <c r="C53" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53">
+        <v>8924</v>
+      </c>
+      <c r="E53">
+        <v>1329</v>
+      </c>
+      <c r="F53">
+        <v>980875.75320000004</v>
+      </c>
+      <c r="G53">
+        <v>88378.436799999996</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>26</v>
+      </c>
+      <c r="C54" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54">
+        <v>9747</v>
+      </c>
+      <c r="E54">
+        <v>1397</v>
+      </c>
+      <c r="F54">
+        <v>1056305.0381</v>
+      </c>
+      <c r="G54">
+        <v>88616.076799999995</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>26</v>
+      </c>
+      <c r="C55" t="s">
+        <v>16</v>
+      </c>
+      <c r="D55">
+        <v>8991</v>
+      </c>
+      <c r="E55">
+        <v>1235</v>
+      </c>
+      <c r="F55">
+        <v>1204729.2156</v>
+      </c>
+      <c r="G55">
+        <v>101348.4984</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>26</v>
+      </c>
+      <c r="C56" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56">
+        <v>8916</v>
+      </c>
+      <c r="E56">
+        <v>1165</v>
+      </c>
+      <c r="F56">
+        <v>1278475.8359000001</v>
+      </c>
+      <c r="G56">
+        <v>77048.550900000002</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57">
+        <v>8317</v>
+      </c>
+      <c r="E57">
+        <v>1019</v>
+      </c>
+      <c r="F57">
+        <v>1138887.6118000001</v>
+      </c>
+      <c r="G57">
+        <v>85378.528600000005</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>26</v>
+      </c>
+      <c r="C58" t="s">
+        <v>19</v>
+      </c>
+      <c r="D58">
+        <v>10543</v>
+      </c>
+      <c r="E58">
+        <v>1315</v>
+      </c>
+      <c r="F58">
+        <v>1355577.7394000001</v>
+      </c>
+      <c r="G58">
+        <v>98554.660600000003</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" t="s">
+        <v>20</v>
+      </c>
+      <c r="D59">
+        <v>8696</v>
+      </c>
+      <c r="E59">
+        <v>1135</v>
+      </c>
+      <c r="F59">
+        <v>1038415.0607</v>
+      </c>
+      <c r="G59">
+        <v>79949.105599999995</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>26</v>
+      </c>
+      <c r="C60" t="s">
+        <v>21</v>
+      </c>
+      <c r="D60">
+        <v>10628</v>
+      </c>
+      <c r="E60">
+        <v>1516</v>
+      </c>
+      <c r="F60">
+        <v>1284769.4339999999</v>
+      </c>
+      <c r="G60">
+        <v>101190.56600000001</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>26</v>
+      </c>
+      <c r="C61" t="s">
+        <v>22</v>
+      </c>
+      <c r="D61">
+        <v>7240</v>
+      </c>
+      <c r="E61">
+        <v>1077</v>
+      </c>
+      <c r="F61">
+        <v>880941.68830000004</v>
+      </c>
+      <c r="G61">
+        <v>69881.205199999997</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Estan todas las distribuidoras
</commit_message>
<xml_diff>
--- a/Data_rechazos_historicos.xlsx
+++ b/Data_rechazos_historicos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="28">
   <si>
     <t>Distribuidora</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>VIACONSUMO</t>
+  </si>
+  <si>
+    <t>ZV</t>
   </si>
 </sst>
 </file>
@@ -160,8 +163,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B3:G61" totalsRowShown="0">
-  <autoFilter ref="B3:G61"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B3:G77" totalsRowShown="0">
+  <autoFilter ref="B3:G77"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Distribuidora"/>
     <tableColumn id="2" name="MES"/>
@@ -437,7 +440,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G61"/>
+  <dimension ref="B3:G77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1630,6 +1633,326 @@
         <v>69881.205199999997</v>
       </c>
     </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>27</v>
+      </c>
+      <c r="C62" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62">
+        <v>4714</v>
+      </c>
+      <c r="E62">
+        <v>191</v>
+      </c>
+      <c r="F62">
+        <v>831072.88359999994</v>
+      </c>
+      <c r="G62">
+        <v>11320.438</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>27</v>
+      </c>
+      <c r="C63" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63">
+        <v>3871</v>
+      </c>
+      <c r="E63">
+        <v>129</v>
+      </c>
+      <c r="F63">
+        <v>713605.09459999995</v>
+      </c>
+      <c r="G63">
+        <v>7362.2052000000003</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>27</v>
+      </c>
+      <c r="C64" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64">
+        <v>3636</v>
+      </c>
+      <c r="E64">
+        <v>129</v>
+      </c>
+      <c r="F64">
+        <v>604788.12150000001</v>
+      </c>
+      <c r="G64">
+        <v>6582.7501000000002</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C65" t="s">
+        <v>10</v>
+      </c>
+      <c r="D65">
+        <v>4218</v>
+      </c>
+      <c r="E65">
+        <v>173</v>
+      </c>
+      <c r="F65">
+        <v>650873.3517</v>
+      </c>
+      <c r="G65">
+        <v>10276.0908</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>27</v>
+      </c>
+      <c r="C66" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66">
+        <v>4168</v>
+      </c>
+      <c r="E66">
+        <v>203</v>
+      </c>
+      <c r="F66">
+        <v>612009.20880000002</v>
+      </c>
+      <c r="G66">
+        <v>9432.9871999999996</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>27</v>
+      </c>
+      <c r="C67" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67">
+        <v>4580</v>
+      </c>
+      <c r="E67">
+        <v>181</v>
+      </c>
+      <c r="F67">
+        <v>732486.26870000002</v>
+      </c>
+      <c r="G67">
+        <v>8934.3811000000005</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>27</v>
+      </c>
+      <c r="C68" t="s">
+        <v>13</v>
+      </c>
+      <c r="D68">
+        <v>4817</v>
+      </c>
+      <c r="E68">
+        <v>193</v>
+      </c>
+      <c r="F68">
+        <v>770206.76729999995</v>
+      </c>
+      <c r="G68">
+        <v>8869.8184000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>27</v>
+      </c>
+      <c r="C69" t="s">
+        <v>14</v>
+      </c>
+      <c r="D69">
+        <v>4818</v>
+      </c>
+      <c r="E69">
+        <v>175</v>
+      </c>
+      <c r="F69">
+        <v>809280.39919999999</v>
+      </c>
+      <c r="G69">
+        <v>8307.0923000000003</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C70" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70">
+        <v>5187</v>
+      </c>
+      <c r="E70">
+        <v>182</v>
+      </c>
+      <c r="F70">
+        <v>879773.26650000003</v>
+      </c>
+      <c r="G70">
+        <v>9466.6821</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>27</v>
+      </c>
+      <c r="C71" t="s">
+        <v>16</v>
+      </c>
+      <c r="D71">
+        <v>4893</v>
+      </c>
+      <c r="E71">
+        <v>177</v>
+      </c>
+      <c r="F71">
+        <v>765758.50650000002</v>
+      </c>
+      <c r="G71">
+        <v>8912.4038999999993</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>27</v>
+      </c>
+      <c r="C72" t="s">
+        <v>17</v>
+      </c>
+      <c r="D72">
+        <v>4678</v>
+      </c>
+      <c r="E72">
+        <v>189</v>
+      </c>
+      <c r="F72">
+        <v>755234.00179999997</v>
+      </c>
+      <c r="G72">
+        <v>10290.7323</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>27</v>
+      </c>
+      <c r="C73" t="s">
+        <v>18</v>
+      </c>
+      <c r="D73">
+        <v>4132</v>
+      </c>
+      <c r="E73">
+        <v>167</v>
+      </c>
+      <c r="F73">
+        <v>698037.77060000005</v>
+      </c>
+      <c r="G73">
+        <v>10579.5489</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>27</v>
+      </c>
+      <c r="C74" t="s">
+        <v>19</v>
+      </c>
+      <c r="D74">
+        <v>4469</v>
+      </c>
+      <c r="E74">
+        <v>170</v>
+      </c>
+      <c r="F74">
+        <v>756851.92139999999</v>
+      </c>
+      <c r="G74">
+        <v>11560.4812</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>27</v>
+      </c>
+      <c r="C75" t="s">
+        <v>20</v>
+      </c>
+      <c r="D75">
+        <v>2510</v>
+      </c>
+      <c r="E75">
+        <v>87</v>
+      </c>
+      <c r="F75">
+        <v>400874.0601</v>
+      </c>
+      <c r="G75">
+        <v>7578.5415000000003</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>27</v>
+      </c>
+      <c r="C76" t="s">
+        <v>21</v>
+      </c>
+      <c r="D76">
+        <v>2301</v>
+      </c>
+      <c r="E76">
+        <v>123</v>
+      </c>
+      <c r="F76">
+        <v>411856.27360000001</v>
+      </c>
+      <c r="G76">
+        <v>8555.5319999999992</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>27</v>
+      </c>
+      <c r="C77" t="s">
+        <v>22</v>
+      </c>
+      <c r="D77">
+        <v>1490</v>
+      </c>
+      <c r="E77">
+        <v>303</v>
+      </c>
+      <c r="F77">
+        <v>311004.18589999998</v>
+      </c>
+      <c r="G77">
+        <v>22993.235000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>